<commit_message>
L_02b military tax, tax_fop_02e
</commit_message>
<xml_diff>
--- a/Tax/data/L_02b.xlsx
+++ b/Tax/data/L_02b.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\Py\Tax\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C043902-D876-41F2-86AD-5D63746D496F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88BB454-0188-490B-A8AD-C5CE133A34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="4260" windowWidth="28365" windowHeight="16305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12225" yWindow="1395" windowWidth="24465" windowHeight="16740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="FOP" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>.</t>
   </si>
@@ -58,6 +58,9 @@
     <t>tax pay</t>
   </si>
   <si>
+    <t>military</t>
+  </si>
+  <si>
     <t>01_2022</t>
   </si>
   <si>
@@ -92,6 +95,15 @@
   </si>
   <si>
     <t>02_2024</t>
+  </si>
+  <si>
+    <t>03_2024</t>
+  </si>
+  <si>
+    <t>04_2024</t>
+  </si>
+  <si>
+    <t>01_2025</t>
   </si>
 </sst>
 </file>
@@ -222,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,9 +264,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -265,10 +274,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -600,32 +613,32 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:BV38"/>
+  <dimension ref="A1:BW37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,38 +658,42 @@
         <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>9165</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="J3" s="24"/>
+      <c r="K3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>15000</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4">
@@ -688,23 +705,24 @@
       <c r="I4">
         <v>1600</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="L4">
+      <c r="J4" s="24"/>
+      <c r="K4" s="10"/>
+      <c r="M4">
         <v>84750</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>2900</v>
       </c>
-      <c r="O4" s="10">
+      <c r="P4" s="10">
         <v>1337.5</v>
       </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>23168.32</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="9">
         <v>15100</v>
@@ -721,35 +739,36 @@
         <f>H4</f>
         <v>1800</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5">
         <f>H5-I5</f>
         <v>755</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="10"/>
+      <c r="L5">
         <v>106334.03</v>
       </c>
-      <c r="L5">
-        <f>L4+K5</f>
+      <c r="M5">
+        <f>M4+L5</f>
         <v>191084.03</v>
       </c>
-      <c r="M5" s="12">
-        <f>L5*0.05</f>
+      <c r="N5" s="12">
+        <f>M5*0.05</f>
         <v>9554.201500000001</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>4237.5</v>
       </c>
-      <c r="O5" s="13">
-        <f>M5-N5</f>
+      <c r="P5" s="13">
+        <f>N5-O5</f>
         <v>5316.701500000001</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>23400</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="9">
         <v>70560</v>
@@ -766,37 +785,38 @@
         <f>H5</f>
         <v>2555</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6">
         <f>H6-I6</f>
         <v>3528</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="10"/>
+      <c r="L6">
         <v>80850</v>
       </c>
-      <c r="L6">
-        <f>L5+K6</f>
+      <c r="M6">
+        <f>M5+L6</f>
         <v>271934.03000000003</v>
       </c>
-      <c r="M6" s="12">
-        <f>L6*0.05</f>
+      <c r="N6" s="12">
+        <f>M6*0.05</f>
         <v>13596.701500000003</v>
       </c>
-      <c r="N6" s="14">
-        <f>M5</f>
+      <c r="O6" s="14">
+        <f>N5</f>
         <v>9554.201500000001</v>
       </c>
-      <c r="O6" s="13">
-        <f>M6-N6</f>
+      <c r="P6" s="13">
+        <f>N6-O6</f>
         <v>4042.5000000000018</v>
       </c>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="B7" s="15">
         <f>SUM(B3:B6)</f>
         <v>70733.320000000007</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="9">
         <v>54000</v>
@@ -811,31 +831,32 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7">
         <f>G7*0.05</f>
         <v>2700</v>
       </c>
-      <c r="K7">
-        <v>81580</v>
-      </c>
+      <c r="K7" s="10"/>
       <c r="L7">
         <v>81580</v>
       </c>
-      <c r="M7" s="11">
-        <f>L7*0.05</f>
+      <c r="M7">
+        <v>81580</v>
+      </c>
+      <c r="N7" s="11">
+        <f>M7*0.05</f>
         <v>4079</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0</v>
       </c>
-      <c r="O7" s="10">
-        <f>L7*0.05</f>
+      <c r="P7" s="10">
+        <f>M7*0.05</f>
         <v>4079</v>
       </c>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="E8" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="9">
         <v>58500</v>
@@ -852,73 +873,75 @@
         <f>H7</f>
         <v>2700</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8">
         <f>H8-I8</f>
         <v>2925</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="10"/>
+      <c r="L8">
         <v>75228.36</v>
       </c>
-      <c r="L8">
-        <f>L7+K8</f>
+      <c r="M8">
+        <f>M7+L8</f>
         <v>156808.35999999999</v>
       </c>
-      <c r="M8" s="12">
-        <f>L8*0.05</f>
+      <c r="N8" s="12">
+        <f>M8*0.05</f>
         <v>7840.4179999999997</v>
       </c>
-      <c r="N8">
-        <f>M7</f>
+      <c r="O8">
+        <f>N7</f>
         <v>4079</v>
       </c>
-      <c r="O8" s="13">
-        <f>M8-N8</f>
+      <c r="P8" s="13">
+        <f>N8-O8</f>
         <v>3761.4179999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:74" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="18">
         <v>61500</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="25">
         <v>174000</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="25">
         <v>8700</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="25">
         <v>5625</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="25">
         <v>3075</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="10"/>
+      <c r="L9" s="25">
         <v>4493</v>
       </c>
-      <c r="L9" s="19">
+      <c r="M9" s="25">
         <v>161301.35999999999</v>
       </c>
-      <c r="M9" s="19">
+      <c r="N9" s="25">
         <v>8065.0679999999993</v>
       </c>
-      <c r="N9" s="19">
+      <c r="O9" s="25">
         <v>7840.4179999999997</v>
       </c>
-      <c r="O9" s="20">
+      <c r="P9" s="19">
         <v>224.64999999999961</v>
       </c>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
         <v>44577</v>
       </c>
       <c r="B10">
@@ -927,261 +950,311 @@
       <c r="C10">
         <v>2400</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="E10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="22">
         <v>63000</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="26">
         <v>237000</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="26">
         <v>11850</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="26">
         <v>8700</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="26">
         <v>3150</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K10" s="10"/>
+      <c r="L10" s="26">
         <v>0</v>
       </c>
-      <c r="O10" s="10"/>
-    </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="E11" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="23">
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E11" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="22">
         <v>119592</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="26">
         <v>119592</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="26">
         <v>5979.6</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="26">
         <v>0</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="26">
         <v>5979.6</v>
       </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="25"/>
-    </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="E12" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="K11" s="10"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="23"/>
+    </row>
+    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="22">
         <v>128105</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="26">
         <v>247697</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="26">
         <v>12384.85</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="26">
         <v>5979.6</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="26">
         <v>6405.25</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="25"/>
-      <c r="BR12">
-        <v>10000</v>
-      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="23"/>
       <c r="BS12">
         <v>10000</v>
       </c>
       <c r="BT12">
+        <v>10000</v>
+      </c>
+      <c r="BU12">
         <v>500</v>
       </c>
-      <c r="BU12">
+      <c r="BV12">
         <v>0</v>
       </c>
-      <c r="BV12">
+      <c r="BW12">
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="E13" s="22"/>
-      <c r="F13" s="9"/>
-      <c r="J13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="BR13">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="9">
+        <v>181002</v>
+      </c>
+      <c r="G13">
+        <v>428699</v>
+      </c>
+      <c r="H13">
+        <v>21434.95</v>
+      </c>
+      <c r="I13">
+        <v>12384.85</v>
+      </c>
+      <c r="J13">
+        <v>9050.1</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="BS13">
         <v>654321</v>
       </c>
-      <c r="BS13">
+      <c r="BT13">
         <v>666666</v>
       </c>
-      <c r="BT13">
+      <c r="BU13">
         <v>33333.300000000003</v>
       </c>
-      <c r="BU13">
+      <c r="BV13">
         <v>0</v>
       </c>
-      <c r="BV13">
+      <c r="BW13">
         <v>33333.300000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="E14" s="22"/>
-      <c r="F14" s="9"/>
-      <c r="J14" s="10"/>
-      <c r="O14" s="10"/>
-    </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="J15" s="10"/>
-      <c r="O15" s="10"/>
-    </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="9">
+        <v>162285</v>
+      </c>
+      <c r="G14">
+        <v>590984</v>
+      </c>
+      <c r="H14">
+        <v>29549.200000000001</v>
+      </c>
+      <c r="I14">
+        <v>21434.95</v>
+      </c>
+      <c r="J14">
+        <v>8114.25</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="E15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="9">
+        <v>163231</v>
+      </c>
+      <c r="G15">
+        <v>163231</v>
+      </c>
+      <c r="H15">
+        <v>8161.55</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>8161.55</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1632.31</v>
+      </c>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
-      <c r="J16" s="10"/>
-      <c r="O16" s="10"/>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K16" s="10"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
-      <c r="J17" s="10"/>
-      <c r="O17" s="10"/>
-    </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K17" s="10"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E18" s="8"/>
       <c r="F18" s="9"/>
-      <c r="J18" s="10"/>
-      <c r="O18" s="10"/>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K18" s="10"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E19" s="8"/>
       <c r="F19" s="9"/>
-      <c r="J19" s="10"/>
-      <c r="O19" s="10"/>
-    </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K19" s="10"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
-      <c r="J20" s="10"/>
-      <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K20" s="10"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
-      <c r="J21" s="10"/>
-      <c r="O21" s="10"/>
-    </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K21" s="10"/>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
-      <c r="J22" s="10"/>
-      <c r="O22" s="10"/>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="10"/>
+      <c r="P22" s="10"/>
+    </row>
+    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
-      <c r="J23" s="10"/>
-      <c r="O23" s="10"/>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="10"/>
+      <c r="P23" s="10"/>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
-      <c r="J24" s="10"/>
-      <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K24" s="10"/>
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
-      <c r="J25" s="10"/>
-      <c r="O25" s="10"/>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K25" s="10"/>
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
-      <c r="J26" s="10"/>
-      <c r="O26" s="10"/>
-    </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K26" s="10"/>
+      <c r="P26" s="10"/>
+    </row>
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
-      <c r="J27" s="10"/>
-      <c r="O27" s="10"/>
-    </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K27" s="10"/>
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
-      <c r="J28" s="10"/>
-      <c r="O28" s="10"/>
-    </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K28" s="10"/>
+      <c r="P28" s="10"/>
+    </row>
+    <row r="29" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E29" s="8"/>
       <c r="F29" s="9"/>
-      <c r="J29" s="10"/>
-      <c r="O29" s="10"/>
-    </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K29" s="10"/>
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
-      <c r="J30" s="10"/>
-      <c r="O30" s="10"/>
-    </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K30" s="10"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
-      <c r="J31" s="10"/>
-      <c r="O31" s="10"/>
-    </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K31" s="10"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
-      <c r="J32" s="10"/>
-      <c r="O32" s="10"/>
-    </row>
-    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K32" s="10"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E33" s="8"/>
       <c r="F33" s="9"/>
-      <c r="J33" s="10"/>
-      <c r="O33" s="10"/>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K33" s="10"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E34" s="8"/>
       <c r="F34" s="9"/>
-      <c r="J34" s="10"/>
-      <c r="O34" s="10"/>
-    </row>
-    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K34" s="10"/>
+      <c r="P34" s="10"/>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E35" s="8"/>
       <c r="F35" s="9"/>
-      <c r="J35" s="10"/>
-      <c r="O35" s="10"/>
-    </row>
-    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K35" s="10"/>
+      <c r="P35" s="10"/>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E36" s="8"/>
       <c r="F36" s="9"/>
-      <c r="J36" s="10"/>
-      <c r="O36" s="10"/>
-    </row>
-    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K36" s="10"/>
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E37" s="8"/>
       <c r="F37" s="9"/>
-      <c r="J37" s="10"/>
-      <c r="O37" s="10"/>
-    </row>
-    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="J38" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="P37" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>